<commit_message>
add logger @ try catch error
</commit_message>
<xml_diff>
--- a/results/inter_diseases/inter_diseases_summarized_results.xlsx
+++ b/results/inter_diseases/inter_diseases_summarized_results.xlsx
@@ -406,49 +406,49 @@
         <v>38</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9566105836245447</v>
+        <v>0.9456614763983506</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7507278508618471</v>
+        <v>0.764160804807917</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6653262206872749</v>
+        <v>0.6300585721236154</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4045912476623776</v>
+        <v>0.40520051698084736</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6825713786846015</v>
+        <v>0.7189667125403201</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9277046816551684</v>
+        <v>0.9226740952719986</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5042214557502599</v>
+        <v>0.4993533338563009</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5062986716958906</v>
+        <v>0.519792235780191</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9061509561023409</v>
+        <v>0.8992333249661543</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9500951667126518</v>
+        <v>0.9453061113289208</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3636220163929068</v>
+        <v>0.3306044216323668</v>
       </c>
       <c r="O4" t="n">
-        <v>0.5590869646954107</v>
+        <v>0.5608009702107111</v>
       </c>
       <c r="P4" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.08258487262045981</v>
+        <v>0.08405355024572106</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1879624922329549</v>
+        <v>0.18321753375134156</v>
       </c>
       <c r="S4" t="n">
         <v>8.0</v>
@@ -457,7 +457,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9052688390343864</v>
+        <v>0.9047657398465535</v>
       </c>
       <c r="V4" t="n">
         <v>3535.0</v>
@@ -466,16 +466,16 @@
         <v>17703.0</v>
       </c>
       <c r="X4" t="n">
-        <v>0.5773687825082233</v>
+        <v>0.579353146404787</v>
       </c>
       <c r="Y4" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.10523640061006609</v>
+        <v>0.10472801220132182</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.28303112466813535</v>
+        <v>0.27794724058069253</v>
       </c>
       <c r="AB4" t="n">
         <v>7.0</v>
@@ -484,7 +484,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.8886973321017287</v>
+        <v>0.8892794859094859</v>
       </c>
       <c r="AE4" t="n">
         <v>5231.0</v>
@@ -504,49 +504,49 @@
         <v>38</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9757504629135114</v>
+        <v>0.9835129865657452</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8789035570707578</v>
+        <v>0.8952815162116312</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4375073095904029</v>
+        <v>0.44776007687756625</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.591823665832272</v>
+        <v>0.5010215729799067</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9420975926248081</v>
+        <v>0.9448570585800264</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6133764230948904</v>
+        <v>0.6212954856145397</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3961078940565673</v>
+        <v>0.37693843812933314</v>
       </c>
       <c r="L5" t="n">
-        <v>0.9552304463275424</v>
+        <v>0.9564806759510953</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9839267347997538</v>
+        <v>0.9790950855338239</v>
       </c>
       <c r="N5" t="n">
-        <v>0.3220936566416087</v>
+        <v>0.29710168709678403</v>
       </c>
       <c r="O5" t="n">
-        <v>0.5737467873159544</v>
+        <v>0.5814996689764491</v>
       </c>
       <c r="P5" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.10769493066606046</v>
+        <v>0.10587633553080246</v>
       </c>
       <c r="R5" t="n">
-        <v>0.29671516253694025</v>
+        <v>0.2972834735167083</v>
       </c>
       <c r="S5" t="n">
         <v>7.0</v>
@@ -555,7 +555,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="U5" t="n">
-        <v>0.8871031171862672</v>
+        <v>0.8881375279109027</v>
       </c>
       <c r="V5" t="n">
         <v>5231.0</v>
@@ -564,16 +564,16 @@
         <v>17596.0</v>
       </c>
       <c r="X5" t="n">
-        <v>0.569648956721479</v>
+        <v>0.546255223675117</v>
       </c>
       <c r="Y5" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.08075699022505115</v>
+        <v>0.08092748351898159</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.19100932030006817</v>
+        <v>0.17984200954762444</v>
       </c>
       <c r="AB5" t="n">
         <v>8.0</v>
@@ -582,7 +582,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.9049310744083858</v>
+        <v>0.9055104461506457</v>
       </c>
       <c r="AE5" t="n">
         <v>3535.0</v>
@@ -602,49 +602,49 @@
         <v>38</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7117707531338336</v>
+        <v>0.6626365911876276</v>
       </c>
       <c r="E6" t="n">
-        <v>0.39082402128576876</v>
+        <v>0.331329879524928</v>
       </c>
       <c r="F6" t="n">
-        <v>0.10950304639187355</v>
+        <v>0.1193344531918586</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5497651256794565</v>
+        <v>0.5275271256297254</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3038572622173041</v>
+        <v>0.3529284614267522</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3035317810155253</v>
+        <v>0.2689452369655388</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7354612986924591</v>
+        <v>0.7185610132659014</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8358877622105704</v>
+        <v>0.8414953449447143</v>
       </c>
       <c r="M6" t="n">
-        <v>0.820033838371163</v>
+        <v>0.8193163197461987</v>
       </c>
       <c r="N6" t="n">
-        <v>0.3524417709612315</v>
+        <v>0.3337481212988949</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8993391951212937</v>
+        <v>0.8956152941874085</v>
       </c>
       <c r="P6" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.07242924394532357</v>
+        <v>0.0709545686574783</v>
       </c>
       <c r="R6" t="n">
-        <v>0.06114230616527706</v>
+        <v>0.06049004594180705</v>
       </c>
       <c r="S6" t="n">
         <v>8.0</v>
@@ -653,7 +653,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9657777166220235</v>
+        <v>0.9659744575512698</v>
       </c>
       <c r="V6" t="n">
         <v>2927.0</v>
@@ -662,16 +662,16 @@
         <v>17631.0</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8705318178504545</v>
+        <v>0.8800787829132712</v>
       </c>
       <c r="Y6" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.07719357949066984</v>
+        <v>0.07503828483920368</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.06584992343032159</v>
+        <v>0.064885712665192</v>
       </c>
       <c r="AB6" t="n">
         <v>8.0</v>
@@ -680,7 +680,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.9650386473787598</v>
+        <v>0.9655308143876321</v>
       </c>
       <c r="AE6" t="n">
         <v>2827.0</v>
@@ -700,49 +700,49 @@
         <v>38</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6759898670932881</v>
+        <v>0.6682737931331699</v>
       </c>
       <c r="E7" t="n">
-        <v>0.20449002136856953</v>
+        <v>0.406961785902004</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1124951347478962</v>
+        <v>0.1289375647210209</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6451151639577865</v>
+        <v>0.6780829262480434</v>
       </c>
       <c r="I7" t="n">
-        <v>0.12926701611560917</v>
+        <v>0.11056506461009344</v>
       </c>
       <c r="J7" t="n">
-        <v>0.11373120655156276</v>
+        <v>0.11129237879680184</v>
       </c>
       <c r="K7" t="n">
-        <v>0.5793460245593635</v>
+        <v>0.552661866571947</v>
       </c>
       <c r="L7" t="n">
-        <v>0.6920344488079596</v>
+        <v>0.7767793988234086</v>
       </c>
       <c r="M7" t="n">
-        <v>0.6964690407090823</v>
+        <v>0.6889427846947838</v>
       </c>
       <c r="N7" t="n">
-        <v>0.30162822878932105</v>
+        <v>0.3032239604725658</v>
       </c>
       <c r="O7" t="n">
-        <v>0.9015365419098366</v>
+        <v>0.8880979786349962</v>
       </c>
       <c r="P7" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.07123816005898702</v>
+        <v>0.07033066757415915</v>
       </c>
       <c r="R7" t="n">
-        <v>0.06125574272588055</v>
+        <v>0.056406329760081676</v>
       </c>
       <c r="S7" t="n">
         <v>8.0</v>
@@ -751,7 +751,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="U7" t="n">
-        <v>0.9659646331002575</v>
+        <v>0.9665268358561148</v>
       </c>
       <c r="V7" t="n">
         <v>2927.0</v>
@@ -760,28 +760,28 @@
         <v>17631.0</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9164856458572457</v>
+        <v>0.9111526360641372</v>
       </c>
       <c r="Y7" t="n">
-        <v>1.6451483562408085</v>
+        <v>1.6445917933215723</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.04662242640803131</v>
+        <v>0.04591344790425954</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.024388860529748736</v>
+        <v>0.025423969145255514</v>
       </c>
       <c r="AB7" t="n">
         <v>8.0</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.4281127363539065</v>
+        <v>0.42831669044222537</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.9784853378186708</v>
+        <v>0.9785843181965108</v>
       </c>
       <c r="AE7" t="n">
-        <v>2803.0</v>
+        <v>2804.0</v>
       </c>
       <c r="AF7" t="n">
         <v>17631.0</v>
@@ -798,49 +798,49 @@
         <v>38</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7248179486999075</v>
+        <v>0.6886531038528473</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5791807526085997</v>
+        <v>0.46935844511449637</v>
       </c>
       <c r="F8" t="n">
-        <v>0.08369777927822468</v>
+        <v>0.1271333407368523</v>
       </c>
       <c r="G8" t="n">
-        <v>0.04127032772726895</v>
+        <v>0.041297978361178246</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5870487817476914</v>
+        <v>0.5613665082025558</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5934898354169992</v>
+        <v>0.4317093735121331</v>
       </c>
       <c r="J8" t="n">
-        <v>0.19588686488138882</v>
+        <v>0.47789919204875425</v>
       </c>
       <c r="K8" t="n">
-        <v>0.7167947679817571</v>
+        <v>0.7570737314844932</v>
       </c>
       <c r="L8" t="n">
-        <v>0.7590408578056302</v>
+        <v>0.8001354136059016</v>
       </c>
       <c r="M8" t="n">
-        <v>0.6995942976027183</v>
+        <v>0.674390956963079</v>
       </c>
       <c r="N8" t="n">
-        <v>0.28611611590124014</v>
+        <v>0.2917088292051539</v>
       </c>
       <c r="O8" t="n">
-        <v>0.8964573079217641</v>
+        <v>0.893843658390407</v>
       </c>
       <c r="P8" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.07794610847692841</v>
+        <v>0.07783046143171042</v>
       </c>
       <c r="R8" t="n">
-        <v>0.06649705100034693</v>
+        <v>0.06464669827685904</v>
       </c>
       <c r="S8" t="n">
         <v>8.0</v>
@@ -849,7 +849,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="U8" t="n">
-        <v>0.9646627096859494</v>
+        <v>0.9646444442435405</v>
       </c>
       <c r="V8" t="n">
         <v>2827.0</v>
@@ -858,16 +858,16 @@
         <v>17294.0</v>
       </c>
       <c r="X8" t="n">
-        <v>0.8729798193838143</v>
+        <v>0.9042582651198517</v>
       </c>
       <c r="Y8" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.07303110905516363</v>
+        <v>0.07291546200994564</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.061292933965537186</v>
+        <v>0.05938475771944027</v>
       </c>
       <c r="AB8" t="n">
         <v>8.0</v>
@@ -876,7 +876,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.9655392943333462</v>
+        <v>0.9655289228439817</v>
       </c>
       <c r="AE8" t="n">
         <v>2927.0</v>
@@ -896,49 +896,49 @@
         <v>38</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6227627190319689</v>
+        <v>0.6282690549949663</v>
       </c>
       <c r="E9" t="n">
-        <v>0.14814805354524638</v>
+        <v>0.20571905396206802</v>
       </c>
       <c r="F9" t="n">
-        <v>0.062378339745704225</v>
+        <v>0.06798733230848508</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6506290773278361</v>
+        <v>0.6515724169646835</v>
       </c>
       <c r="I9" t="n">
-        <v>0.07065986669927775</v>
+        <v>0.054399304934903775</v>
       </c>
       <c r="J9" t="n">
-        <v>0.09220818694035211</v>
+        <v>0.08095143825577351</v>
       </c>
       <c r="K9" t="n">
-        <v>0.6073698343114758</v>
+        <v>0.6202908502744893</v>
       </c>
       <c r="L9" t="n">
-        <v>0.569449800923465</v>
+        <v>0.5890753603777906</v>
       </c>
       <c r="M9" t="n">
-        <v>0.5635701528253685</v>
+        <v>0.5787165633163235</v>
       </c>
       <c r="N9" t="n">
-        <v>0.16409069426094822</v>
+        <v>0.2642573420549294</v>
       </c>
       <c r="O9" t="n">
-        <v>0.8976654177026535</v>
+        <v>0.8905269355950052</v>
       </c>
       <c r="P9" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.07742569677344743</v>
+        <v>0.07858216722562739</v>
       </c>
       <c r="R9" t="n">
-        <v>0.06800046258818088</v>
+        <v>0.06635249219382447</v>
       </c>
       <c r="S9" t="n">
         <v>8.0</v>
@@ -947,7 +947,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="U9" t="n">
-        <v>0.964695742932859</v>
+        <v>0.9644770076124555</v>
       </c>
       <c r="V9" t="n">
         <v>2827.0</v>
@@ -956,16 +956,16 @@
         <v>17294.0</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9211999693123131</v>
+        <v>0.9164430436532871</v>
       </c>
       <c r="Y9" t="n">
-        <v>1.6448547923467098</v>
+        <v>1.6449558843640575</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.047241817971550824</v>
+        <v>0.04712617092633283</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.02503758528969585</v>
+        <v>0.024921938244477852</v>
       </c>
       <c r="AB9" t="n">
         <v>8.0</v>
@@ -974,7 +974,7 @@
         <v>0.42796005706134094</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.9780908446309168</v>
+        <v>0.9782073990352628</v>
       </c>
       <c r="AE9" t="n">
         <v>2804.0</v>
@@ -994,76 +994,76 @@
         <v>38</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6937469987582208</v>
+        <v>0.673618062865532</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5236358125696138</v>
+        <v>0.539479157676884</v>
       </c>
       <c r="F10" t="n">
-        <v>0.48179986991916784</v>
+        <v>0.1077650153751142</v>
       </c>
       <c r="G10" t="n">
-        <v>0.05008788908619872</v>
+        <v>0.05191784502367472</v>
       </c>
       <c r="H10" t="n">
-        <v>0.5665508878668899</v>
+        <v>0.5820473919560439</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1960909016974193</v>
+        <v>0.22681397051781618</v>
       </c>
       <c r="J10" t="n">
-        <v>0.13148347452111772</v>
+        <v>0.12218702164325645</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7645657712919358</v>
+        <v>0.7586315204410721</v>
       </c>
       <c r="L10" t="n">
-        <v>0.792699061490167</v>
+        <v>0.7994515125391964</v>
       </c>
       <c r="M10" t="n">
-        <v>0.7626646100601947</v>
+        <v>0.7491156745951816</v>
       </c>
       <c r="N10" t="n">
-        <v>0.29958261011136855</v>
+        <v>0.33650525491247707</v>
       </c>
       <c r="O10" t="n">
-        <v>0.9221351017723327</v>
+        <v>0.9107468577455363</v>
       </c>
       <c r="P10" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6449992268231095</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.04758418740849195</v>
+        <v>0.04780943799977475</v>
       </c>
       <c r="R10" t="n">
-        <v>0.025791192701880843</v>
+        <v>0.02607275594098435</v>
       </c>
       <c r="S10" t="n">
         <v>8.0</v>
       </c>
       <c r="T10" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.42806140664048553</v>
       </c>
       <c r="U10" t="n">
-        <v>0.978323523908231</v>
+        <v>0.9782217217725766</v>
       </c>
       <c r="V10" t="n">
-        <v>2806.0</v>
+        <v>2801.0</v>
       </c>
       <c r="W10" t="n">
         <v>17758.0</v>
       </c>
       <c r="X10" t="n">
-        <v>0.8985035060941358</v>
+        <v>0.8761406687344427</v>
       </c>
       <c r="Y10" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.07039080977587567</v>
+        <v>0.07101024890190337</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.06062056537898412</v>
+        <v>0.06132447347674287</v>
       </c>
       <c r="AB10" t="n">
         <v>8.0</v>
@@ -1072,7 +1072,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.9662221077799068</v>
+        <v>0.9663097608114993</v>
       </c>
       <c r="AE10" t="n">
         <v>2927.0</v>
@@ -1092,58 +1092,58 @@
         <v>38</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6803164653324585</v>
+        <v>0.6635296737058404</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5497336753958348</v>
+        <v>0.5111500915962837</v>
       </c>
       <c r="F11" t="n">
-        <v>0.17937087071476707</v>
+        <v>0.4220207415339144</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0067174025017321505</v>
+        <v>0.006698734445897117</v>
       </c>
       <c r="H11" t="n">
-        <v>0.5383825109366681</v>
+        <v>0.5248738516037168</v>
       </c>
       <c r="I11" t="n">
-        <v>0.13719028284618176</v>
+        <v>0.14393199591389003</v>
       </c>
       <c r="J11" t="n">
-        <v>0.05702086070396707</v>
+        <v>0.03766206494261239</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7589221305351742</v>
+        <v>0.6066353837327659</v>
       </c>
       <c r="L11" t="n">
-        <v>0.7725215414323146</v>
+        <v>0.7662160270532827</v>
       </c>
       <c r="M11" t="n">
-        <v>0.7067688377836298</v>
+        <v>0.7096485200906893</v>
       </c>
       <c r="N11" t="n">
-        <v>0.3168085570813165</v>
+        <v>0.32171455918727837</v>
       </c>
       <c r="O11" t="n">
-        <v>0.9231524454132581</v>
+        <v>0.9029955643655834</v>
       </c>
       <c r="P11" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6451874590741786</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0474434057889402</v>
+        <v>0.047837594323685104</v>
       </c>
       <c r="R11" t="n">
-        <v>0.02542516049104629</v>
+        <v>0.025833427187746373</v>
       </c>
       <c r="S11" t="n">
         <v>8.0</v>
       </c>
       <c r="T11" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.4280114041339986</v>
       </c>
       <c r="U11" t="n">
-        <v>0.9784063873875082</v>
+        <v>0.9781110971879238</v>
       </c>
       <c r="V11" t="n">
         <v>2806.0</v>
@@ -1152,16 +1152,16 @@
         <v>17758.0</v>
       </c>
       <c r="X11" t="n">
-        <v>0.9223087932910594</v>
+        <v>0.8825180346154053</v>
       </c>
       <c r="Y11" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.07664151368397341</v>
+        <v>0.0755715733753801</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.06180313098321884</v>
+        <v>0.06425273116341931</v>
       </c>
       <c r="AB11" t="n">
         <v>8.0</v>
@@ -1170,7 +1170,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.9656281700763872</v>
+        <v>0.9657130473994732</v>
       </c>
       <c r="AE11" t="n">
         <v>2827.0</v>
@@ -1340,49 +1340,49 @@
         <v>40</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9947305720994657</v>
+        <v>0.9897566378563254</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9990104927387842</v>
+        <v>0.9965738823243689</v>
       </c>
       <c r="F4" t="n">
-        <v>0.979144476043958</v>
+        <v>0.7904466935757164</v>
       </c>
       <c r="G4" t="n">
-        <v>0.006565379206978874</v>
+        <v>-0.026796558296251705</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3840777112744001</v>
+        <v>0.9897678367591095</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9947305720994657</v>
+        <v>0.993163177505839</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9791672303597145</v>
+        <v>0.976339149382084</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3649201962055928</v>
+        <v>0.5482307949371441</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9895022416153192</v>
+        <v>0.9802072433922007</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9947305720994657</v>
+        <v>1.0</v>
       </c>
       <c r="N4" t="n">
-        <v>0.557643298266016</v>
+        <v>0.4302747783423345</v>
       </c>
       <c r="O4" t="n">
-        <v>0.5590869646954107</v>
+        <v>0.5608009702107111</v>
       </c>
       <c r="P4" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.08258487262045981</v>
+        <v>0.08405355024572106</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1879624922329549</v>
+        <v>0.18321753375134156</v>
       </c>
       <c r="S4" t="n">
         <v>8.0</v>
@@ -1391,7 +1391,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9052688390343864</v>
+        <v>0.9047657398465535</v>
       </c>
       <c r="V4" t="n">
         <v>3535.0</v>
@@ -1400,16 +1400,16 @@
         <v>17703.0</v>
       </c>
       <c r="X4" t="n">
-        <v>0.5773687825082233</v>
+        <v>0.579353146404787</v>
       </c>
       <c r="Y4" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.10523640061006609</v>
+        <v>0.10472801220132182</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.28303112466813535</v>
+        <v>0.27794724058069253</v>
       </c>
       <c r="AB4" t="n">
         <v>7.0</v>
@@ -1418,7 +1418,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.8886973321017287</v>
+        <v>0.8892794859094859</v>
       </c>
       <c r="AE4" t="n">
         <v>5231.0</v>
@@ -1438,49 +1438,49 @@
         <v>40</v>
       </c>
       <c r="D5" t="n">
-        <v>0.984944755799888</v>
+        <v>0.9955921371054552</v>
       </c>
       <c r="E5" t="n">
-        <v>0.983275858809821</v>
+        <v>0.9980996074224366</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5709394967469701</v>
+        <v>0.6757598381039323</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6115954716402436</v>
+        <v>0.6641482186334635</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9965049414280559</v>
+        <v>1.0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9965049414280559</v>
+        <v>1.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4620584065436479</v>
+        <v>0.5063172784411563</v>
       </c>
       <c r="L5" t="n">
-        <v>0.9895584647509612</v>
+        <v>0.9890144948983313</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9982493111581865</v>
+        <v>1.0</v>
       </c>
       <c r="N5" t="n">
-        <v>0.28495483099547864</v>
+        <v>0.35248653686192843</v>
       </c>
       <c r="O5" t="n">
-        <v>0.5737467873159544</v>
+        <v>0.5814996689764491</v>
       </c>
       <c r="P5" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.10769493066606046</v>
+        <v>0.10587633553080246</v>
       </c>
       <c r="R5" t="n">
-        <v>0.29671516253694025</v>
+        <v>0.2972834735167083</v>
       </c>
       <c r="S5" t="n">
         <v>7.0</v>
@@ -1489,7 +1489,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="U5" t="n">
-        <v>0.8871031171862672</v>
+        <v>0.8881375279109027</v>
       </c>
       <c r="V5" t="n">
         <v>5231.0</v>
@@ -1498,16 +1498,16 @@
         <v>17596.0</v>
       </c>
       <c r="X5" t="n">
-        <v>0.569648956721479</v>
+        <v>0.546255223675117</v>
       </c>
       <c r="Y5" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.08075699022505115</v>
+        <v>0.08092748351898159</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.19100932030006817</v>
+        <v>0.17984200954762444</v>
       </c>
       <c r="AB5" t="n">
         <v>8.0</v>
@@ -1516,7 +1516,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.9049310744083858</v>
+        <v>0.9055104461506457</v>
       </c>
       <c r="AE5" t="n">
         <v>3535.0</v>
@@ -1536,49 +1536,49 @@
         <v>40</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8058490736026824</v>
+        <v>0.8295065566850656</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6236353679221224</v>
+        <v>0.7851836121751987</v>
       </c>
       <c r="F6" t="n">
-        <v>0.34936222011504847</v>
+        <v>0.5422572214371782</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6670979860161131</v>
+        <v>0.6951296680262711</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9016462315501194</v>
+        <v>0.9089749077947432</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8108218135459341</v>
+        <v>0.8671510478248629</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8783083308589826</v>
+        <v>0.8528408802591506</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8820273062930675</v>
+        <v>0.9158139151610982</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8860341526781551</v>
+        <v>0.8875511502236305</v>
       </c>
       <c r="N6" t="n">
-        <v>0.5303572766809216</v>
+        <v>0.4672463404876779</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8993391951212937</v>
+        <v>0.8956152941874085</v>
       </c>
       <c r="P6" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.07242924394532357</v>
+        <v>0.0709545686574783</v>
       </c>
       <c r="R6" t="n">
-        <v>0.06114230616527706</v>
+        <v>0.06049004594180705</v>
       </c>
       <c r="S6" t="n">
         <v>8.0</v>
@@ -1587,7 +1587,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9657777166220235</v>
+        <v>0.9659744575512698</v>
       </c>
       <c r="V6" t="n">
         <v>2927.0</v>
@@ -1596,16 +1596,16 @@
         <v>17631.0</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8705318178504545</v>
+        <v>0.8800787829132712</v>
       </c>
       <c r="Y6" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.07719357949066984</v>
+        <v>0.07503828483920368</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.06584992343032159</v>
+        <v>0.064885712665192</v>
       </c>
       <c r="AB6" t="n">
         <v>8.0</v>
@@ -1614,7 +1614,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.9650386473787598</v>
+        <v>0.9655308143876321</v>
       </c>
       <c r="AE6" t="n">
         <v>2827.0</v>
@@ -1634,49 +1634,49 @@
         <v>40</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8189809982042083</v>
+        <v>0.6286762012741722</v>
       </c>
       <c r="E7" t="n">
-        <v>0.42660989976921093</v>
+        <v>0.8300880945717218</v>
       </c>
       <c r="F7" t="n">
-        <v>0.517129535315432</v>
+        <v>0.1495172743772414</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9198720895781612</v>
+        <v>0.9395347097628668</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9585853433408633</v>
+        <v>0.9110623628956441</v>
       </c>
       <c r="J7" t="n">
-        <v>0.915263011849097</v>
+        <v>0.787689301851545</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8705514866928402</v>
+        <v>0.9382053037855448</v>
       </c>
       <c r="L7" t="n">
-        <v>0.48537690908565984</v>
+        <v>0.3134160090191657</v>
       </c>
       <c r="M7" t="n">
-        <v>0.7695543615612254</v>
+        <v>0.6649102464042814</v>
       </c>
       <c r="N7" t="n">
-        <v>0.3979891235832422</v>
+        <v>0.2024062153946608</v>
       </c>
       <c r="O7" t="n">
-        <v>0.9015365419098366</v>
+        <v>0.8880979786349962</v>
       </c>
       <c r="P7" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.07123816005898702</v>
+        <v>0.07033066757415915</v>
       </c>
       <c r="R7" t="n">
-        <v>0.06125574272588055</v>
+        <v>0.056406329760081676</v>
       </c>
       <c r="S7" t="n">
         <v>8.0</v>
@@ -1685,7 +1685,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="U7" t="n">
-        <v>0.9659646331002575</v>
+        <v>0.9665268358561148</v>
       </c>
       <c r="V7" t="n">
         <v>2927.0</v>
@@ -1694,28 +1694,28 @@
         <v>17631.0</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9164856458572457</v>
+        <v>0.9111526360641372</v>
       </c>
       <c r="Y7" t="n">
-        <v>1.6451483562408085</v>
+        <v>1.6445917933215723</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.04662242640803131</v>
+        <v>0.04591344790425954</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.024388860529748736</v>
+        <v>0.025423969145255514</v>
       </c>
       <c r="AB7" t="n">
         <v>8.0</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.4281127363539065</v>
+        <v>0.42831669044222537</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.9784853378186708</v>
+        <v>0.9785843181965108</v>
       </c>
       <c r="AE7" t="n">
-        <v>2803.0</v>
+        <v>2804.0</v>
       </c>
       <c r="AF7" t="n">
         <v>17631.0</v>
@@ -1750,7 +1750,7 @@
         <v>0.0</v>
       </c>
       <c r="J8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K8" t="n">
         <v>0.0</v>
@@ -1765,16 +1765,16 @@
         <v>0.0</v>
       </c>
       <c r="O8" t="n">
-        <v>0.8964573079217641</v>
+        <v>0.893843658390407</v>
       </c>
       <c r="P8" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.07794610847692841</v>
+        <v>0.07783046143171042</v>
       </c>
       <c r="R8" t="n">
-        <v>0.06649705100034693</v>
+        <v>0.06464669827685904</v>
       </c>
       <c r="S8" t="n">
         <v>8.0</v>
@@ -1783,7 +1783,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="U8" t="n">
-        <v>0.9646627096859494</v>
+        <v>0.9646444442435405</v>
       </c>
       <c r="V8" t="n">
         <v>2827.0</v>
@@ -1792,16 +1792,16 @@
         <v>17294.0</v>
       </c>
       <c r="X8" t="n">
-        <v>0.8729798193838143</v>
+        <v>0.9042582651198517</v>
       </c>
       <c r="Y8" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.07303110905516363</v>
+        <v>0.07291546200994564</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.061292933965537186</v>
+        <v>0.05938475771944027</v>
       </c>
       <c r="AB8" t="n">
         <v>8.0</v>
@@ -1810,7 +1810,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.9655392943333462</v>
+        <v>0.9655289228439817</v>
       </c>
       <c r="AE8" t="n">
         <v>2927.0</v>
@@ -1830,49 +1830,49 @@
         <v>40</v>
       </c>
       <c r="D9" t="n">
-        <v>0.566192727151607</v>
+        <v>0.45897740784780017</v>
       </c>
       <c r="E9" t="n">
-        <v>0.30435096111295645</v>
+        <v>0.45090510148107515</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4682139557202956</v>
+        <v>0.18202247191011234</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5210286216768971</v>
+        <v>0.25851851851851854</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8504622931175146</v>
+        <v>0.7612940833576217</v>
       </c>
       <c r="J9" t="n">
-        <v>0.8656547087831813</v>
+        <v>0.7671310776229742</v>
       </c>
       <c r="K9" t="n">
-        <v>0.29753618202925175</v>
+        <v>0.6793168880455408</v>
       </c>
       <c r="L9" t="n">
-        <v>0.8893770594696375</v>
+        <v>0.5521885521885521</v>
       </c>
       <c r="M9" t="n">
-        <v>0.7543984776356776</v>
+        <v>0.7004936917169501</v>
       </c>
       <c r="N9" t="n">
-        <v>0.04383197926973558</v>
+        <v>0.12062645784738421</v>
       </c>
       <c r="O9" t="n">
-        <v>0.8976654177026535</v>
+        <v>0.8905269355950052</v>
       </c>
       <c r="P9" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.07742569677344743</v>
+        <v>0.07858216722562739</v>
       </c>
       <c r="R9" t="n">
-        <v>0.06800046258818088</v>
+        <v>0.06635249219382447</v>
       </c>
       <c r="S9" t="n">
         <v>8.0</v>
@@ -1881,7 +1881,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="U9" t="n">
-        <v>0.964695742932859</v>
+        <v>0.9644770076124555</v>
       </c>
       <c r="V9" t="n">
         <v>2827.0</v>
@@ -1890,16 +1890,16 @@
         <v>17294.0</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9211999693123131</v>
+        <v>0.9164430436532871</v>
       </c>
       <c r="Y9" t="n">
-        <v>1.6448547923467098</v>
+        <v>1.6449558843640575</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.047241817971550824</v>
+        <v>0.04712617092633283</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.02503758528969585</v>
+        <v>0.024921938244477852</v>
       </c>
       <c r="AB9" t="n">
         <v>8.0</v>
@@ -1908,7 +1908,7 @@
         <v>0.42796005706134094</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.9780908446309168</v>
+        <v>0.9782073990352628</v>
       </c>
       <c r="AE9" t="n">
         <v>2804.0</v>
@@ -1931,7 +1931,7 @@
         <v>1.0</v>
       </c>
       <c r="E10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F10" t="n">
         <v>1.0</v>
@@ -1940,64 +1940,64 @@
         <v>0.0</v>
       </c>
       <c r="H10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N10" t="n">
         <v>1.0</v>
       </c>
       <c r="O10" t="n">
-        <v>0.9221351017723327</v>
+        <v>0.9107468577455363</v>
       </c>
       <c r="P10" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6449992268231095</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.04758418740849195</v>
+        <v>0.04780943799977475</v>
       </c>
       <c r="R10" t="n">
-        <v>0.025791192701880843</v>
+        <v>0.02607275594098435</v>
       </c>
       <c r="S10" t="n">
         <v>8.0</v>
       </c>
       <c r="T10" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.42806140664048553</v>
       </c>
       <c r="U10" t="n">
-        <v>0.978323523908231</v>
+        <v>0.9782217217725766</v>
       </c>
       <c r="V10" t="n">
-        <v>2806.0</v>
+        <v>2801.0</v>
       </c>
       <c r="W10" t="n">
         <v>17758.0</v>
       </c>
       <c r="X10" t="n">
-        <v>0.8985035060941358</v>
+        <v>0.8761406687344427</v>
       </c>
       <c r="Y10" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.07039080977587567</v>
+        <v>0.07101024890190337</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.06062056537898412</v>
+        <v>0.06132447347674287</v>
       </c>
       <c r="AB10" t="n">
         <v>8.0</v>
@@ -2006,7 +2006,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.9662221077799068</v>
+        <v>0.9663097608114993</v>
       </c>
       <c r="AE10" t="n">
         <v>2927.0</v>
@@ -2037,25 +2037,25 @@
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11" t="n">
-        <v>0.9231524454132581</v>
+        <v>0.9029955643655834</v>
       </c>
       <c r="P11" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6451874590741786</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0474434057889402</v>
+        <v>0.047837594323685104</v>
       </c>
       <c r="R11" t="n">
-        <v>0.02542516049104629</v>
+        <v>0.025833427187746373</v>
       </c>
       <c r="S11" t="n">
         <v>8.0</v>
       </c>
       <c r="T11" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.4280114041339986</v>
       </c>
       <c r="U11" t="n">
-        <v>0.9784063873875082</v>
+        <v>0.9781110971879238</v>
       </c>
       <c r="V11" t="n">
         <v>2806.0</v>
@@ -2064,16 +2064,16 @@
         <v>17758.0</v>
       </c>
       <c r="X11" t="n">
-        <v>0.9223087932910594</v>
+        <v>0.8825180346154053</v>
       </c>
       <c r="Y11" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.07664151368397341</v>
+        <v>0.0755715733753801</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.06180313098321884</v>
+        <v>0.06425273116341931</v>
       </c>
       <c r="AB11" t="n">
         <v>8.0</v>
@@ -2082,7 +2082,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.9656281700763872</v>
+        <v>0.9657130473994732</v>
       </c>
       <c r="AE11" t="n">
         <v>2827.0</v>
@@ -2252,49 +2252,49 @@
         <v>42</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9533837635105818</v>
+        <v>0.9418459684565201</v>
       </c>
       <c r="E4" t="n">
-        <v>0.701191905520503</v>
+        <v>0.7144309440500036</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6277225392131478</v>
+        <v>0.6148534194846098</v>
       </c>
       <c r="G4" t="n">
-        <v>0.34733618405936045</v>
+        <v>0.34105189859666485</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6698516517291832</v>
+        <v>0.6673281015674591</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9208650066234902</v>
+        <v>0.9160515611554785</v>
       </c>
       <c r="J4" t="n">
-        <v>0.40934765307927956</v>
+        <v>0.40164148499826785</v>
       </c>
       <c r="K4" t="n">
-        <v>0.46112203865461965</v>
+        <v>0.46638399702865607</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8985936592649968</v>
+        <v>0.896688048171714</v>
       </c>
       <c r="M4" t="n">
-        <v>0.948163670306067</v>
+        <v>0.9416201432610288</v>
       </c>
       <c r="N4" t="n">
-        <v>0.31884899504797376</v>
+        <v>0.31728233491950897</v>
       </c>
       <c r="O4" t="n">
-        <v>0.5590869646954107</v>
+        <v>0.5608009702107111</v>
       </c>
       <c r="P4" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.08258487262045981</v>
+        <v>0.08405355024572106</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1879624922329549</v>
+        <v>0.18321753375134156</v>
       </c>
       <c r="S4" t="n">
         <v>8.0</v>
@@ -2303,7 +2303,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9052688390343864</v>
+        <v>0.9047657398465535</v>
       </c>
       <c r="V4" t="n">
         <v>3535.0</v>
@@ -2312,16 +2312,16 @@
         <v>17703.0</v>
       </c>
       <c r="X4" t="n">
-        <v>0.5773687825082233</v>
+        <v>0.579353146404787</v>
       </c>
       <c r="Y4" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.10523640061006609</v>
+        <v>0.10472801220132182</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.28303112466813535</v>
+        <v>0.27794724058069253</v>
       </c>
       <c r="AB4" t="n">
         <v>7.0</v>
@@ -2330,7 +2330,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.8886973321017287</v>
+        <v>0.8892794859094859</v>
       </c>
       <c r="AE4" t="n">
         <v>5231.0</v>
@@ -2350,49 +2350,49 @@
         <v>42</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9681646372368553</v>
+        <v>0.9766371626104556</v>
       </c>
       <c r="E5" t="n">
-        <v>0.791739363706205</v>
+        <v>0.8283356673670743</v>
       </c>
       <c r="F5" t="n">
-        <v>0.575196280916216</v>
+        <v>0.5022069002053624</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5917671670882095</v>
+        <v>0.42469980623275</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8860382759809399</v>
+        <v>0.9039354596490901</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2921603940508051</v>
+        <v>0.4107641316041396</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3638554944638432</v>
+        <v>0.3314263629129823</v>
       </c>
       <c r="L5" t="n">
-        <v>0.9281109455249205</v>
+        <v>0.9376072159756274</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9724231057159102</v>
+        <v>0.9673821043730982</v>
       </c>
       <c r="N5" t="n">
-        <v>0.3938442092114672</v>
+        <v>0.31643704885254326</v>
       </c>
       <c r="O5" t="n">
-        <v>0.5737467873159544</v>
+        <v>0.5814996689764491</v>
       </c>
       <c r="P5" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.10769493066606046</v>
+        <v>0.10587633553080246</v>
       </c>
       <c r="R5" t="n">
-        <v>0.29671516253694025</v>
+        <v>0.2972834735167083</v>
       </c>
       <c r="S5" t="n">
         <v>7.0</v>
@@ -2401,7 +2401,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="U5" t="n">
-        <v>0.8871031171862672</v>
+        <v>0.8881375279109027</v>
       </c>
       <c r="V5" t="n">
         <v>5231.0</v>
@@ -2410,16 +2410,16 @@
         <v>17596.0</v>
       </c>
       <c r="X5" t="n">
-        <v>0.569648956721479</v>
+        <v>0.546255223675117</v>
       </c>
       <c r="Y5" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.08075699022505115</v>
+        <v>0.08092748351898159</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.19100932030006817</v>
+        <v>0.17984200954762444</v>
       </c>
       <c r="AB5" t="n">
         <v>8.0</v>
@@ -2428,7 +2428,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.9049310744083858</v>
+        <v>0.9055104461506457</v>
       </c>
       <c r="AE5" t="n">
         <v>3535.0</v>
@@ -2448,49 +2448,49 @@
         <v>42</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6951603073344843</v>
+        <v>0.64248915081971</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3571389525405061</v>
+        <v>0.28529870852195244</v>
       </c>
       <c r="F6" t="n">
-        <v>0.08856065798890714</v>
+        <v>0.10607013025288836</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5233902301557622</v>
+        <v>0.5077772168890387</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2125964158448716</v>
+        <v>0.28966030118229685</v>
       </c>
       <c r="J6" t="n">
-        <v>0.24384156212548713</v>
+        <v>0.2301489213965843</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7102979022382729</v>
+        <v>0.6999354672678589</v>
       </c>
       <c r="L6" t="n">
-        <v>0.829916903941165</v>
+        <v>0.8313056117592997</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8093087834301665</v>
+        <v>0.8092505952652082</v>
       </c>
       <c r="N6" t="n">
-        <v>0.3171381236979108</v>
+        <v>0.31864169932221176</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8993391951212937</v>
+        <v>0.8956152941874085</v>
       </c>
       <c r="P6" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.07242924394532357</v>
+        <v>0.0709545686574783</v>
       </c>
       <c r="R6" t="n">
-        <v>0.06114230616527706</v>
+        <v>0.06049004594180705</v>
       </c>
       <c r="S6" t="n">
         <v>8.0</v>
@@ -2499,7 +2499,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9657777166220235</v>
+        <v>0.9659744575512698</v>
       </c>
       <c r="V6" t="n">
         <v>2927.0</v>
@@ -2508,16 +2508,16 @@
         <v>17631.0</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8705318178504545</v>
+        <v>0.8800787829132712</v>
       </c>
       <c r="Y6" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.07719357949066984</v>
+        <v>0.07503828483920368</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.06584992343032159</v>
+        <v>0.064885712665192</v>
       </c>
       <c r="AB6" t="n">
         <v>8.0</v>
@@ -2526,7 +2526,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.9650386473787598</v>
+        <v>0.9655308143876321</v>
       </c>
       <c r="AE6" t="n">
         <v>2827.0</v>
@@ -2546,49 +2546,49 @@
         <v>42</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6699959059717181</v>
+        <v>0.6578443697998935</v>
       </c>
       <c r="E7" t="n">
-        <v>0.18763013231311926</v>
+        <v>0.3850412433507304</v>
       </c>
       <c r="F7" t="n">
-        <v>0.09802492971796468</v>
+        <v>0.11326734108387122</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6328084400429634</v>
+        <v>0.6641857781713675</v>
       </c>
       <c r="I7" t="n">
-        <v>0.10427117945036832</v>
+        <v>0.07124001875050129</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0932551294349235</v>
+        <v>0.07382333447581876</v>
       </c>
       <c r="K7" t="n">
-        <v>0.5652819802592611</v>
+        <v>0.5318969867031349</v>
       </c>
       <c r="L7" t="n">
-        <v>0.6987364187027904</v>
+        <v>0.7827420184826056</v>
       </c>
       <c r="M7" t="n">
-        <v>0.6911135406238108</v>
+        <v>0.6851602307729446</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2922012848815663</v>
+        <v>0.28901032961618284</v>
       </c>
       <c r="O7" t="n">
-        <v>0.9015365419098366</v>
+        <v>0.8880979786349962</v>
       </c>
       <c r="P7" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.07123816005898702</v>
+        <v>0.07033066757415915</v>
       </c>
       <c r="R7" t="n">
-        <v>0.06125574272588055</v>
+        <v>0.056406329760081676</v>
       </c>
       <c r="S7" t="n">
         <v>8.0</v>
@@ -2597,7 +2597,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="U7" t="n">
-        <v>0.9659646331002575</v>
+        <v>0.9665268358561148</v>
       </c>
       <c r="V7" t="n">
         <v>2927.0</v>
@@ -2606,28 +2606,28 @@
         <v>17631.0</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9164856458572457</v>
+        <v>0.9111526360641372</v>
       </c>
       <c r="Y7" t="n">
-        <v>1.6451483562408085</v>
+        <v>1.6445917933215723</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.04662242640803131</v>
+        <v>0.04591344790425954</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.024388860529748736</v>
+        <v>0.025423969145255514</v>
       </c>
       <c r="AB7" t="n">
         <v>8.0</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.4281127363539065</v>
+        <v>0.42831669044222537</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.9784853378186708</v>
+        <v>0.9785843181965108</v>
       </c>
       <c r="AE7" t="n">
-        <v>2803.0</v>
+        <v>2804.0</v>
       </c>
       <c r="AF7" t="n">
         <v>17631.0</v>
@@ -2644,49 +2644,49 @@
         <v>42</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7265573577396927</v>
+        <v>0.6894414215019746</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5804470431825077</v>
+        <v>0.47048666781093934</v>
       </c>
       <c r="F8" t="n">
-        <v>0.08137210884105689</v>
+        <v>0.12569651546715702</v>
       </c>
       <c r="G8" t="n">
-        <v>0.03659526030644227</v>
+        <v>0.03761641611436244</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5872521244076631</v>
+        <v>0.561738153603977</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5939188030938309</v>
+        <v>0.43124186739153464</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1927645692591469</v>
+        <v>0.47737267376545833</v>
       </c>
       <c r="K8" t="n">
-        <v>0.7168170661039412</v>
+        <v>0.7575752249192274</v>
       </c>
       <c r="L8" t="n">
-        <v>0.7606517599272544</v>
+        <v>0.8012547881496335</v>
       </c>
       <c r="M8" t="n">
-        <v>0.7005555484449243</v>
+        <v>0.6754610542064371</v>
       </c>
       <c r="N8" t="n">
-        <v>0.2860111464012098</v>
+        <v>0.29199127326964164</v>
       </c>
       <c r="O8" t="n">
-        <v>0.8964573079217641</v>
+        <v>0.893843658390407</v>
       </c>
       <c r="P8" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.07794610847692841</v>
+        <v>0.07783046143171042</v>
       </c>
       <c r="R8" t="n">
-        <v>0.06649705100034693</v>
+        <v>0.06464669827685904</v>
       </c>
       <c r="S8" t="n">
         <v>8.0</v>
@@ -2695,7 +2695,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="U8" t="n">
-        <v>0.9646627096859494</v>
+        <v>0.9646444442435405</v>
       </c>
       <c r="V8" t="n">
         <v>2827.0</v>
@@ -2704,16 +2704,16 @@
         <v>17294.0</v>
       </c>
       <c r="X8" t="n">
-        <v>0.8729798193838143</v>
+        <v>0.9042582651198517</v>
       </c>
       <c r="Y8" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.07303110905516363</v>
+        <v>0.07291546200994564</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.061292933965537186</v>
+        <v>0.05938475771944027</v>
       </c>
       <c r="AB8" t="n">
         <v>8.0</v>
@@ -2722,7 +2722,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.9655392943333462</v>
+        <v>0.9655289228439817</v>
       </c>
       <c r="AE8" t="n">
         <v>2927.0</v>
@@ -2742,49 +2742,49 @@
         <v>42</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6086413832626385</v>
+        <v>0.6290135447654258</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1305030639379928</v>
+        <v>0.20413177812978556</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0445308832597053</v>
+        <v>0.06848012806255843</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6446671843234351</v>
+        <v>0.6536835076957438</v>
       </c>
       <c r="I9" t="n">
-        <v>0.064938924859324</v>
+        <v>0.053917272011193514</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0576380894841773</v>
+        <v>0.0781092541816872</v>
       </c>
       <c r="K9" t="n">
-        <v>0.6147950089730978</v>
+        <v>0.62008313595231</v>
       </c>
       <c r="L9" t="n">
-        <v>0.5400779614120726</v>
+        <v>0.5888523285380969</v>
       </c>
       <c r="M9" t="n">
-        <v>0.5318749360634948</v>
+        <v>0.5780548167787636</v>
       </c>
       <c r="N9" t="n">
-        <v>0.16516992654486248</v>
+        <v>0.26469574767423715</v>
       </c>
       <c r="O9" t="n">
-        <v>0.8976654177026535</v>
+        <v>0.8905269355950052</v>
       </c>
       <c r="P9" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.07742569677344743</v>
+        <v>0.07858216722562739</v>
       </c>
       <c r="R9" t="n">
-        <v>0.06800046258818088</v>
+        <v>0.06635249219382447</v>
       </c>
       <c r="S9" t="n">
         <v>8.0</v>
@@ -2793,7 +2793,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="U9" t="n">
-        <v>0.964695742932859</v>
+        <v>0.9644770076124555</v>
       </c>
       <c r="V9" t="n">
         <v>2827.0</v>
@@ -2802,16 +2802,16 @@
         <v>17294.0</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9211999693123131</v>
+        <v>0.9164430436532871</v>
       </c>
       <c r="Y9" t="n">
-        <v>1.6448547923467098</v>
+        <v>1.6449558843640575</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.047241817971550824</v>
+        <v>0.04712617092633283</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.02503758528969585</v>
+        <v>0.024921938244477852</v>
       </c>
       <c r="AB9" t="n">
         <v>8.0</v>
@@ -2820,7 +2820,7 @@
         <v>0.42796005706134094</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.9780908446309168</v>
+        <v>0.9782073990352628</v>
       </c>
       <c r="AE9" t="n">
         <v>2804.0</v>
@@ -2840,76 +2840,76 @@
         <v>42</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6948303853947563</v>
+        <v>0.6744076970830113</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5232169222528458</v>
+        <v>0.5393602126338529</v>
       </c>
       <c r="F10" t="n">
-        <v>0.48347487989279064</v>
+        <v>0.10756488747265115</v>
       </c>
       <c r="G10" t="n">
-        <v>0.04875834369146831</v>
+        <v>0.050944511350917654</v>
       </c>
       <c r="H10" t="n">
-        <v>0.5663797292178591</v>
+        <v>0.5822471781593247</v>
       </c>
       <c r="I10" t="n">
-        <v>0.19524638392125207</v>
+        <v>0.22643857130775402</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1305769069518738</v>
+        <v>0.12157965517496817</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7644467603876433</v>
+        <v>0.7589519249453349</v>
       </c>
       <c r="L10" t="n">
-        <v>0.7928020429480291</v>
+        <v>0.7998295004169774</v>
       </c>
       <c r="M10" t="n">
-        <v>0.762590157188071</v>
+        <v>0.7493947598203765</v>
       </c>
       <c r="N10" t="n">
-        <v>0.2993436083821317</v>
+        <v>0.33635986907259624</v>
       </c>
       <c r="O10" t="n">
-        <v>0.9221351017723327</v>
+        <v>0.9107468577455363</v>
       </c>
       <c r="P10" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6449992268231095</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.04758418740849195</v>
+        <v>0.04780943799977475</v>
       </c>
       <c r="R10" t="n">
-        <v>0.025791192701880843</v>
+        <v>0.02607275594098435</v>
       </c>
       <c r="S10" t="n">
         <v>8.0</v>
       </c>
       <c r="T10" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.42806140664048553</v>
       </c>
       <c r="U10" t="n">
-        <v>0.978323523908231</v>
+        <v>0.9782217217725766</v>
       </c>
       <c r="V10" t="n">
-        <v>2806.0</v>
+        <v>2801.0</v>
       </c>
       <c r="W10" t="n">
         <v>17758.0</v>
       </c>
       <c r="X10" t="n">
-        <v>0.8985035060941358</v>
+        <v>0.8761406687344427</v>
       </c>
       <c r="Y10" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.07039080977587567</v>
+        <v>0.07101024890190337</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.06062056537898412</v>
+        <v>0.06132447347674287</v>
       </c>
       <c r="AB10" t="n">
         <v>8.0</v>
@@ -2918,7 +2918,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.9662221077799068</v>
+        <v>0.9663097608114993</v>
       </c>
       <c r="AE10" t="n">
         <v>2927.0</v>
@@ -2938,58 +2938,58 @@
         <v>42</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6803164653324585</v>
+        <v>0.6635296737058404</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5497336753958348</v>
+        <v>0.5111500915962837</v>
       </c>
       <c r="F11" t="n">
-        <v>0.17937087071476707</v>
+        <v>0.4220207415339144</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0067174025017321505</v>
+        <v>0.006698734445897117</v>
       </c>
       <c r="H11" t="n">
-        <v>0.5383825109366681</v>
+        <v>0.5248738516037168</v>
       </c>
       <c r="I11" t="n">
-        <v>0.13719028284618176</v>
+        <v>0.14393199591389003</v>
       </c>
       <c r="J11" t="n">
-        <v>0.05702086070396707</v>
+        <v>0.03766206494261239</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7589221305351742</v>
+        <v>0.6066353837327659</v>
       </c>
       <c r="L11" t="n">
-        <v>0.7725215414323146</v>
+        <v>0.7662160270532827</v>
       </c>
       <c r="M11" t="n">
-        <v>0.7067688377836298</v>
+        <v>0.7096485200906893</v>
       </c>
       <c r="N11" t="n">
-        <v>0.3168085570813165</v>
+        <v>0.32171455918727837</v>
       </c>
       <c r="O11" t="n">
-        <v>0.9231524454132581</v>
+        <v>0.9029955643655834</v>
       </c>
       <c r="P11" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6451874590741786</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0474434057889402</v>
+        <v>0.047837594323685104</v>
       </c>
       <c r="R11" t="n">
-        <v>0.02542516049104629</v>
+        <v>0.025833427187746373</v>
       </c>
       <c r="S11" t="n">
         <v>8.0</v>
       </c>
       <c r="T11" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.4280114041339986</v>
       </c>
       <c r="U11" t="n">
-        <v>0.9784063873875082</v>
+        <v>0.9781110971879238</v>
       </c>
       <c r="V11" t="n">
         <v>2806.0</v>
@@ -2998,16 +2998,16 @@
         <v>17758.0</v>
       </c>
       <c r="X11" t="n">
-        <v>0.9223087932910594</v>
+        <v>0.8825180346154053</v>
       </c>
       <c r="Y11" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.07664151368397341</v>
+        <v>0.0755715733753801</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.06180313098321884</v>
+        <v>0.06425273116341931</v>
       </c>
       <c r="AB11" t="n">
         <v>8.0</v>
@@ -3016,7 +3016,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.9656281700763872</v>
+        <v>0.9657130473994732</v>
       </c>
       <c r="AE11" t="n">
         <v>2827.0</v>
@@ -3170,37 +3170,37 @@
         <v>45</v>
       </c>
       <c r="D4" t="n">
-        <v>0.006499713247944944</v>
+        <v>0.007455553431466259</v>
       </c>
       <c r="E4" t="n">
-        <v>0.14261135538138023</v>
+        <v>0.1340087937296884</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1846683234563181</v>
+        <v>0.14184668323456318</v>
       </c>
       <c r="G4" t="n">
-        <v>0.07359969413114127</v>
+        <v>0.06996750143376028</v>
       </c>
       <c r="H4" t="n">
-        <v>0.35308736379277383</v>
+        <v>0.35996941311412733</v>
       </c>
       <c r="I4" t="n">
         <v>0.0015293442936341044</v>
       </c>
       <c r="J4" t="n">
-        <v>0.005543873064423628</v>
+        <v>0.0045880328809023135</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5590869646954107</v>
+        <v>0.5608009702107111</v>
       </c>
       <c r="L4" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="M4" t="n">
-        <v>0.08258487262045981</v>
+        <v>0.08405355024572106</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1879624922329549</v>
+        <v>0.18321753375134156</v>
       </c>
       <c r="O4" t="n">
         <v>8.0</v>
@@ -3209,7 +3209,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9052688390343864</v>
+        <v>0.9047657398465535</v>
       </c>
       <c r="R4" t="n">
         <v>3535.0</v>
@@ -3218,16 +3218,16 @@
         <v>17703.0</v>
       </c>
       <c r="T4" t="n">
-        <v>0.5773687825082233</v>
+        <v>0.579353146404787</v>
       </c>
       <c r="U4" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="V4" t="n">
-        <v>0.10523640061006609</v>
+        <v>0.10472801220132182</v>
       </c>
       <c r="W4" t="n">
-        <v>0.28303112466813535</v>
+        <v>0.27794724058069253</v>
       </c>
       <c r="X4" t="n">
         <v>7.0</v>
@@ -3236,7 +3236,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.8886973321017287</v>
+        <v>0.8892794859094859</v>
       </c>
       <c r="AA4" t="n">
         <v>5231.0</v>
@@ -3268,7 +3268,7 @@
         <v>7.0</v>
       </c>
       <c r="H5" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="I5" t="n">
         <v>8.0</v>
@@ -3277,16 +3277,16 @@
         <v>8.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.5590869646954107</v>
+        <v>0.5608009702107111</v>
       </c>
       <c r="L5" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="M5" t="n">
-        <v>0.08258487262045981</v>
+        <v>0.08405355024572106</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1879624922329549</v>
+        <v>0.18321753375134156</v>
       </c>
       <c r="O5" t="n">
         <v>8.0</v>
@@ -3295,7 +3295,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.9052688390343864</v>
+        <v>0.9047657398465535</v>
       </c>
       <c r="R5" t="n">
         <v>3535.0</v>
@@ -3304,16 +3304,16 @@
         <v>17703.0</v>
       </c>
       <c r="T5" t="n">
-        <v>0.5773687825082233</v>
+        <v>0.579353146404787</v>
       </c>
       <c r="U5" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="V5" t="n">
-        <v>0.10523640061006609</v>
+        <v>0.10472801220132182</v>
       </c>
       <c r="W5" t="n">
-        <v>0.28303112466813535</v>
+        <v>0.27794724058069253</v>
       </c>
       <c r="X5" t="n">
         <v>7.0</v>
@@ -3322,7 +3322,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.8886973321017287</v>
+        <v>0.8892794859094859</v>
       </c>
       <c r="AA5" t="n">
         <v>5231.0</v>
@@ -3342,37 +3342,37 @@
         <v>47</v>
       </c>
       <c r="D6" t="n">
-        <v>0.41406996750143377</v>
+        <v>0.4117759510609826</v>
       </c>
       <c r="E6" t="n">
-        <v>0.31886828522271077</v>
+        <v>0.32919135920474096</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3446759701777863</v>
+        <v>0.3368380806729115</v>
       </c>
       <c r="G6" t="n">
-        <v>0.40948193462053145</v>
+        <v>0.41349646339132096</v>
       </c>
       <c r="H6" t="n">
-        <v>0.35308736379277383</v>
+        <v>0.35996941311412733</v>
       </c>
       <c r="I6" t="n">
-        <v>0.43376027528197286</v>
+        <v>0.42706939399732363</v>
       </c>
       <c r="J6" t="n">
-        <v>0.41731982412540625</v>
+        <v>0.4133052953546167</v>
       </c>
       <c r="K6" t="n">
-        <v>0.5590869646954107</v>
+        <v>0.5608009702107111</v>
       </c>
       <c r="L6" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="M6" t="n">
-        <v>0.08258487262045981</v>
+        <v>0.08405355024572106</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1879624922329549</v>
+        <v>0.18321753375134156</v>
       </c>
       <c r="O6" t="n">
         <v>8.0</v>
@@ -3381,7 +3381,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.9052688390343864</v>
+        <v>0.9047657398465535</v>
       </c>
       <c r="R6" t="n">
         <v>3535.0</v>
@@ -3390,16 +3390,16 @@
         <v>17703.0</v>
       </c>
       <c r="T6" t="n">
-        <v>0.5773687825082233</v>
+        <v>0.579353146404787</v>
       </c>
       <c r="U6" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="V6" t="n">
-        <v>0.10523640061006609</v>
+        <v>0.10472801220132182</v>
       </c>
       <c r="W6" t="n">
-        <v>0.28303112466813535</v>
+        <v>0.27794724058069253</v>
       </c>
       <c r="X6" t="n">
         <v>7.0</v>
@@ -3408,7 +3408,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.8886973321017287</v>
+        <v>0.8892794859094859</v>
       </c>
       <c r="AA6" t="n">
         <v>5231.0</v>
@@ -3431,16 +3431,16 @@
         <v>0.0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.06704384724186704</v>
+        <v>0.058557284299858556</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2466760961810467</v>
+        <v>0.36124469589816127</v>
       </c>
       <c r="G7" t="n">
-        <v>0.05205091937765205</v>
+        <v>0.05431400282885431</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3094766619519095</v>
+        <v>0.3057991513437058</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
@@ -3449,16 +3449,16 @@
         <v>0.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.5737467873159544</v>
+        <v>0.5814996689764491</v>
       </c>
       <c r="L7" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="M7" t="n">
-        <v>0.10769493066606046</v>
+        <v>0.10587633553080246</v>
       </c>
       <c r="N7" t="n">
-        <v>0.29671516253694025</v>
+        <v>0.2972834735167083</v>
       </c>
       <c r="O7" t="n">
         <v>7.0</v>
@@ -3467,7 +3467,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.8871031171862672</v>
+        <v>0.8881375279109027</v>
       </c>
       <c r="R7" t="n">
         <v>5231.0</v>
@@ -3476,16 +3476,16 @@
         <v>17596.0</v>
       </c>
       <c r="T7" t="n">
-        <v>0.569648956721479</v>
+        <v>0.546255223675117</v>
       </c>
       <c r="U7" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="V7" t="n">
-        <v>0.08075699022505115</v>
+        <v>0.08092748351898159</v>
       </c>
       <c r="W7" t="n">
-        <v>0.19100932030006817</v>
+        <v>0.17984200954762444</v>
       </c>
       <c r="X7" t="n">
         <v>8.0</v>
@@ -3494,7 +3494,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.9049310744083858</v>
+        <v>0.9055104461506457</v>
       </c>
       <c r="AA7" t="n">
         <v>3535.0</v>
@@ -3526,7 +3526,7 @@
         <v>8.0</v>
       </c>
       <c r="H8" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="I8" t="n">
         <v>7.0</v>
@@ -3535,16 +3535,16 @@
         <v>7.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.5737467873159544</v>
+        <v>0.5814996689764491</v>
       </c>
       <c r="L8" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="M8" t="n">
-        <v>0.10769493066606046</v>
+        <v>0.10587633553080246</v>
       </c>
       <c r="N8" t="n">
-        <v>0.29671516253694025</v>
+        <v>0.2972834735167083</v>
       </c>
       <c r="O8" t="n">
         <v>7.0</v>
@@ -3553,7 +3553,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.8871031171862672</v>
+        <v>0.8881375279109027</v>
       </c>
       <c r="R8" t="n">
         <v>5231.0</v>
@@ -3562,16 +3562,16 @@
         <v>17596.0</v>
       </c>
       <c r="T8" t="n">
-        <v>0.569648956721479</v>
+        <v>0.546255223675117</v>
       </c>
       <c r="U8" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="V8" t="n">
-        <v>0.08075699022505115</v>
+        <v>0.08092748351898159</v>
       </c>
       <c r="W8" t="n">
-        <v>0.19100932030006817</v>
+        <v>0.17984200954762444</v>
       </c>
       <c r="X8" t="n">
         <v>8.0</v>
@@ -3580,7 +3580,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.9049310744083858</v>
+        <v>0.9055104461506457</v>
       </c>
       <c r="AA8" t="n">
         <v>3535.0</v>
@@ -3600,37 +3600,37 @@
         <v>47</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4933521923620934</v>
+        <v>0.4958981612446959</v>
       </c>
       <c r="E9" t="n">
-        <v>0.45035360678925035</v>
+        <v>0.4562942008486563</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2466760961810467</v>
+        <v>0.36124469589816127</v>
       </c>
       <c r="G9" t="n">
-        <v>0.47553041018387554</v>
+        <v>0.47835926449787836</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4229137199434229</v>
+        <v>0.42234794908062234</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5024045261669025</v>
+        <v>0.5012729844413013</v>
       </c>
       <c r="J9" t="n">
-        <v>0.49165487977369166</v>
+        <v>0.4896746817538897</v>
       </c>
       <c r="K9" t="n">
-        <v>0.5737467873159544</v>
+        <v>0.5814996689764491</v>
       </c>
       <c r="L9" t="n">
         <v>1.6177899474534594</v>
       </c>
       <c r="M9" t="n">
-        <v>0.10769493066606046</v>
+        <v>0.10587633553080246</v>
       </c>
       <c r="N9" t="n">
-        <v>0.29671516253694025</v>
+        <v>0.2972834735167083</v>
       </c>
       <c r="O9" t="n">
         <v>7.0</v>
@@ -3639,7 +3639,7 @@
         <v>0.4240107054100554</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.8871031171862672</v>
+        <v>0.8881375279109027</v>
       </c>
       <c r="R9" t="n">
         <v>5231.0</v>
@@ -3648,16 +3648,16 @@
         <v>17596.0</v>
       </c>
       <c r="T9" t="n">
-        <v>0.569648956721479</v>
+        <v>0.546255223675117</v>
       </c>
       <c r="U9" t="n">
         <v>1.3572155246905484</v>
       </c>
       <c r="V9" t="n">
-        <v>0.08075699022505115</v>
+        <v>0.08092748351898159</v>
       </c>
       <c r="W9" t="n">
-        <v>0.19100932030006817</v>
+        <v>0.17984200954762444</v>
       </c>
       <c r="X9" t="n">
         <v>8.0</v>
@@ -3666,7 +3666,7 @@
         <v>0.4947666195190948</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.9049310744083858</v>
+        <v>0.9055104461506457</v>
       </c>
       <c r="AA9" t="n">
         <v>3535.0</v>
@@ -3689,34 +3689,34 @@
         <v>0.0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.22178988326848248</v>
+        <v>0.304209409267775</v>
       </c>
       <c r="F10" t="n">
-        <v>0.45065440396179696</v>
+        <v>0.5224619738238415</v>
       </c>
       <c r="G10" t="n">
-        <v>0.42589317297488505</v>
+        <v>0.43190661478599224</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4736469755925009</v>
+        <v>0.4764768305624337</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0010611956137247967</v>
+        <v>7.074637424831977E-4</v>
       </c>
       <c r="J10" t="n">
         <v>0.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8993391951212937</v>
+        <v>0.8956152941874085</v>
       </c>
       <c r="L10" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="M10" t="n">
-        <v>0.07242924394532357</v>
+        <v>0.0709545686574783</v>
       </c>
       <c r="N10" t="n">
-        <v>0.06114230616527706</v>
+        <v>0.06049004594180705</v>
       </c>
       <c r="O10" t="n">
         <v>8.0</v>
@@ -3725,7 +3725,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.9657777166220235</v>
+        <v>0.9659744575512698</v>
       </c>
       <c r="R10" t="n">
         <v>2927.0</v>
@@ -3734,16 +3734,16 @@
         <v>17631.0</v>
       </c>
       <c r="T10" t="n">
-        <v>0.8705318178504545</v>
+        <v>0.8800787829132712</v>
       </c>
       <c r="U10" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="V10" t="n">
-        <v>0.07719357949066984</v>
+        <v>0.07503828483920368</v>
       </c>
       <c r="W10" t="n">
-        <v>0.06584992343032159</v>
+        <v>0.064885712665192</v>
       </c>
       <c r="X10" t="n">
         <v>8.0</v>
@@ -3752,7 +3752,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.9650386473787598</v>
+        <v>0.9655308143876321</v>
       </c>
       <c r="AA10" t="n">
         <v>2827.0</v>
@@ -3781,10 +3781,10 @@
         <v>9.0</v>
       </c>
       <c r="G11" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="H11" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="I11" t="n">
         <v>9.0</v>
@@ -3793,16 +3793,16 @@
         <v>8.0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.8993391951212937</v>
+        <v>0.8956152941874085</v>
       </c>
       <c r="L11" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="M11" t="n">
-        <v>0.07242924394532357</v>
+        <v>0.0709545686574783</v>
       </c>
       <c r="N11" t="n">
-        <v>0.06114230616527706</v>
+        <v>0.06049004594180705</v>
       </c>
       <c r="O11" t="n">
         <v>8.0</v>
@@ -3811,7 +3811,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.9657777166220235</v>
+        <v>0.9659744575512698</v>
       </c>
       <c r="R11" t="n">
         <v>2927.0</v>
@@ -3820,16 +3820,16 @@
         <v>17631.0</v>
       </c>
       <c r="T11" t="n">
-        <v>0.8705318178504545</v>
+        <v>0.8800787829132712</v>
       </c>
       <c r="U11" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="V11" t="n">
-        <v>0.07719357949066984</v>
+        <v>0.07503828483920368</v>
       </c>
       <c r="W11" t="n">
-        <v>0.06584992343032159</v>
+        <v>0.064885712665192</v>
       </c>
       <c r="X11" t="n">
         <v>8.0</v>
@@ -3838,7 +3838,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.9650386473787598</v>
+        <v>0.9655308143876321</v>
       </c>
       <c r="AA11" t="n">
         <v>2827.0</v>
@@ -3858,37 +3858,37 @@
         <v>47</v>
       </c>
       <c r="D12" t="n">
-        <v>0.41917226742129465</v>
+        <v>0.4039617969579059</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2553944110364344</v>
+        <v>0.304209409267775</v>
       </c>
       <c r="F12" t="n">
-        <v>0.45065440396179696</v>
+        <v>0.5224619738238415</v>
       </c>
       <c r="G12" t="n">
-        <v>0.42589317297488505</v>
+        <v>0.43190661478599224</v>
       </c>
       <c r="H12" t="n">
-        <v>0.4736469755925009</v>
+        <v>0.4764768305624337</v>
       </c>
       <c r="I12" t="n">
-        <v>0.4372125928546162</v>
+        <v>0.4396887159533074</v>
       </c>
       <c r="J12" t="n">
-        <v>0.43261407852847544</v>
+        <v>0.4280155642023346</v>
       </c>
       <c r="K12" t="n">
-        <v>0.8993391951212937</v>
+        <v>0.8956152941874085</v>
       </c>
       <c r="L12" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="M12" t="n">
-        <v>0.07242924394532357</v>
+        <v>0.0709545686574783</v>
       </c>
       <c r="N12" t="n">
-        <v>0.06114230616527706</v>
+        <v>0.06049004594180705</v>
       </c>
       <c r="O12" t="n">
         <v>8.0</v>
@@ -3897,7 +3897,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.9657777166220235</v>
+        <v>0.9659744575512698</v>
       </c>
       <c r="R12" t="n">
         <v>2927.0</v>
@@ -3906,16 +3906,16 @@
         <v>17631.0</v>
       </c>
       <c r="T12" t="n">
-        <v>0.8705318178504545</v>
+        <v>0.8800787829132712</v>
       </c>
       <c r="U12" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="V12" t="n">
-        <v>0.07719357949066984</v>
+        <v>0.07503828483920368</v>
       </c>
       <c r="W12" t="n">
-        <v>0.06584992343032159</v>
+        <v>0.064885712665192</v>
       </c>
       <c r="X12" t="n">
         <v>8.0</v>
@@ -3924,7 +3924,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.9650386473787598</v>
+        <v>0.9655308143876321</v>
       </c>
       <c r="AA12" t="n">
         <v>2827.0</v>
@@ -3947,16 +3947,16 @@
         <v>0.0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.326792722083482</v>
+        <v>0.2888730385164051</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4641455583303603</v>
+        <v>0.36554921540656204</v>
       </c>
       <c r="G13" t="n">
-        <v>0.7021048876204067</v>
+        <v>0.6722539229671898</v>
       </c>
       <c r="H13" t="n">
-        <v>0.8091330717088834</v>
+        <v>0.8830242510699001</v>
       </c>
       <c r="I13" t="n">
         <v>0.0</v>
@@ -3965,16 +3965,16 @@
         <v>0.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.9015365419098366</v>
+        <v>0.8880979786349962</v>
       </c>
       <c r="L13" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="M13" t="n">
-        <v>0.07123816005898702</v>
+        <v>0.07033066757415915</v>
       </c>
       <c r="N13" t="n">
-        <v>0.06125574272588055</v>
+        <v>0.056406329760081676</v>
       </c>
       <c r="O13" t="n">
         <v>8.0</v>
@@ -3983,7 +3983,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.9659646331002575</v>
+        <v>0.9665268358561148</v>
       </c>
       <c r="R13" t="n">
         <v>2927.0</v>
@@ -3992,28 +3992,28 @@
         <v>17631.0</v>
       </c>
       <c r="T13" t="n">
-        <v>0.9164856458572457</v>
+        <v>0.9111526360641372</v>
       </c>
       <c r="U13" t="n">
-        <v>1.6451483562408085</v>
+        <v>1.6445917933215723</v>
       </c>
       <c r="V13" t="n">
-        <v>0.04662242640803131</v>
+        <v>0.04591344790425954</v>
       </c>
       <c r="W13" t="n">
-        <v>0.024388860529748736</v>
+        <v>0.025423969145255514</v>
       </c>
       <c r="X13" t="n">
         <v>8.0</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.4281127363539065</v>
+        <v>0.42831669044222537</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.9784853378186708</v>
+        <v>0.9785843181965108</v>
       </c>
       <c r="AA13" t="n">
-        <v>2803.0</v>
+        <v>2804.0</v>
       </c>
       <c r="AB13" t="n">
         <v>17631.0</v>
@@ -4042,25 +4042,25 @@
         <v>9.0</v>
       </c>
       <c r="H14" t="n">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="I14" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="J14" t="n">
         <v>8.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.9015365419098366</v>
+        <v>0.8880979786349962</v>
       </c>
       <c r="L14" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="M14" t="n">
-        <v>0.07123816005898702</v>
+        <v>0.07033066757415915</v>
       </c>
       <c r="N14" t="n">
-        <v>0.06125574272588055</v>
+        <v>0.056406329760081676</v>
       </c>
       <c r="O14" t="n">
         <v>8.0</v>
@@ -4069,7 +4069,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.9659646331002575</v>
+        <v>0.9665268358561148</v>
       </c>
       <c r="R14" t="n">
         <v>2927.0</v>
@@ -4078,28 +4078,28 @@
         <v>17631.0</v>
       </c>
       <c r="T14" t="n">
-        <v>0.9164856458572457</v>
+        <v>0.9111526360641372</v>
       </c>
       <c r="U14" t="n">
-        <v>1.6451483562408085</v>
+        <v>1.6445917933215723</v>
       </c>
       <c r="V14" t="n">
-        <v>0.04662242640803131</v>
+        <v>0.04591344790425954</v>
       </c>
       <c r="W14" t="n">
-        <v>0.024388860529748736</v>
+        <v>0.025423969145255514</v>
       </c>
       <c r="X14" t="n">
         <v>8.0</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.4281127363539065</v>
+        <v>0.42831669044222537</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.9784853378186708</v>
+        <v>0.9785843181965108</v>
       </c>
       <c r="AA14" t="n">
-        <v>2803.0</v>
+        <v>2804.0</v>
       </c>
       <c r="AB14" t="n">
         <v>17631.0</v>
@@ -4116,37 +4116,37 @@
         <v>47</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5094541562611488</v>
+        <v>0.5106990014265336</v>
       </c>
       <c r="E15" t="n">
-        <v>0.326792722083482</v>
+        <v>0.3455777460770328</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4641455583303603</v>
+        <v>0.36554921540656204</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7021048876204067</v>
+        <v>0.6722539229671898</v>
       </c>
       <c r="H15" t="n">
-        <v>0.8091330717088834</v>
+        <v>0.8830242510699001</v>
       </c>
       <c r="I15" t="n">
-        <v>0.4994648590795576</v>
+        <v>0.4743223965763195</v>
       </c>
       <c r="J15" t="n">
-        <v>0.4666428826257581</v>
+        <v>0.46504992867332384</v>
       </c>
       <c r="K15" t="n">
-        <v>0.9015365419098366</v>
+        <v>0.8880979786349962</v>
       </c>
       <c r="L15" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="M15" t="n">
-        <v>0.07123816005898702</v>
+        <v>0.07033066757415915</v>
       </c>
       <c r="N15" t="n">
-        <v>0.06125574272588055</v>
+        <v>0.056406329760081676</v>
       </c>
       <c r="O15" t="n">
         <v>8.0</v>
@@ -4155,7 +4155,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.9659646331002575</v>
+        <v>0.9665268358561148</v>
       </c>
       <c r="R15" t="n">
         <v>2927.0</v>
@@ -4164,28 +4164,28 @@
         <v>17631.0</v>
       </c>
       <c r="T15" t="n">
-        <v>0.9164856458572457</v>
+        <v>0.9111526360641372</v>
       </c>
       <c r="U15" t="n">
-        <v>1.6451483562408085</v>
+        <v>1.6445917933215723</v>
       </c>
       <c r="V15" t="n">
-        <v>0.04662242640803131</v>
+        <v>0.04591344790425954</v>
       </c>
       <c r="W15" t="n">
-        <v>0.024388860529748736</v>
+        <v>0.025423969145255514</v>
       </c>
       <c r="X15" t="n">
         <v>8.0</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.4281127363539065</v>
+        <v>0.42831669044222537</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.9784853378186708</v>
+        <v>0.9785843181965108</v>
       </c>
       <c r="AA15" t="n">
-        <v>2803.0</v>
+        <v>2804.0</v>
       </c>
       <c r="AB15" t="n">
         <v>17631.0</v>
@@ -4205,34 +4205,34 @@
         <v>0.0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1885889989750598</v>
+        <v>0.2377861291424667</v>
       </c>
       <c r="F16" t="n">
-        <v>0.47762213870857534</v>
+        <v>0.45917321489579777</v>
       </c>
       <c r="G16" t="n">
-        <v>0.28800819952169454</v>
+        <v>0.3652203621455415</v>
       </c>
       <c r="H16" t="n">
-        <v>0.49914588315681585</v>
+        <v>0.2719508028698326</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0013665869490946361</v>
+        <v>3.4164673727365904E-4</v>
       </c>
       <c r="J16" t="n">
         <v>0.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.8964573079217641</v>
+        <v>0.893843658390407</v>
       </c>
       <c r="L16" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="M16" t="n">
-        <v>0.07794610847692841</v>
+        <v>0.07783046143171042</v>
       </c>
       <c r="N16" t="n">
-        <v>0.06649705100034693</v>
+        <v>0.06464669827685904</v>
       </c>
       <c r="O16" t="n">
         <v>8.0</v>
@@ -4241,7 +4241,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.9646627096859494</v>
+        <v>0.9646444442435405</v>
       </c>
       <c r="R16" t="n">
         <v>2827.0</v>
@@ -4250,16 +4250,16 @@
         <v>17294.0</v>
       </c>
       <c r="T16" t="n">
-        <v>0.8729798193838143</v>
+        <v>0.9042582651198517</v>
       </c>
       <c r="U16" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="V16" t="n">
-        <v>0.07303110905516363</v>
+        <v>0.07291546200994564</v>
       </c>
       <c r="W16" t="n">
-        <v>0.061292933965537186</v>
+        <v>0.05938475771944027</v>
       </c>
       <c r="X16" t="n">
         <v>8.0</v>
@@ -4268,7 +4268,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.9655392943333462</v>
+        <v>0.9655289228439817</v>
       </c>
       <c r="AA16" t="n">
         <v>2927.0</v>
@@ -4309,16 +4309,16 @@
         <v>8.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.8964573079217641</v>
+        <v>0.893843658390407</v>
       </c>
       <c r="L17" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="M17" t="n">
-        <v>0.07794610847692841</v>
+        <v>0.07783046143171042</v>
       </c>
       <c r="N17" t="n">
-        <v>0.06649705100034693</v>
+        <v>0.06464669827685904</v>
       </c>
       <c r="O17" t="n">
         <v>8.0</v>
@@ -4327,7 +4327,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.9646627096859494</v>
+        <v>0.9646444442435405</v>
       </c>
       <c r="R17" t="n">
         <v>2827.0</v>
@@ -4336,16 +4336,16 @@
         <v>17294.0</v>
       </c>
       <c r="T17" t="n">
-        <v>0.8729798193838143</v>
+        <v>0.9042582651198517</v>
       </c>
       <c r="U17" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="V17" t="n">
-        <v>0.07303110905516363</v>
+        <v>0.07291546200994564</v>
       </c>
       <c r="W17" t="n">
-        <v>0.061292933965537186</v>
+        <v>0.05938475771944027</v>
       </c>
       <c r="X17" t="n">
         <v>8.0</v>
@@ -4354,7 +4354,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.9655392943333462</v>
+        <v>0.9655289228439817</v>
       </c>
       <c r="AA17" t="n">
         <v>2927.0</v>
@@ -4374,37 +4374,37 @@
         <v>47</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4263751281175265</v>
+        <v>0.3829859924837718</v>
       </c>
       <c r="E18" t="n">
-        <v>0.3918688076528869</v>
+        <v>0.3495046122309532</v>
       </c>
       <c r="F18" t="n">
-        <v>0.47762213870857534</v>
+        <v>0.45917321489579777</v>
       </c>
       <c r="G18" t="n">
-        <v>0.3505295524427742</v>
+        <v>0.3652203621455415</v>
       </c>
       <c r="H18" t="n">
-        <v>0.49914588315681585</v>
+        <v>0.33242227536727026</v>
       </c>
       <c r="I18" t="n">
-        <v>0.45063204646395627</v>
+        <v>0.4332080628629997</v>
       </c>
       <c r="J18" t="n">
-        <v>0.4649812094294499</v>
+        <v>0.45917321489579777</v>
       </c>
       <c r="K18" t="n">
-        <v>0.8964573079217641</v>
+        <v>0.893843658390407</v>
       </c>
       <c r="L18" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="M18" t="n">
-        <v>0.07794610847692841</v>
+        <v>0.07783046143171042</v>
       </c>
       <c r="N18" t="n">
-        <v>0.06649705100034693</v>
+        <v>0.06464669827685904</v>
       </c>
       <c r="O18" t="n">
         <v>8.0</v>
@@ -4413,7 +4413,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.9646627096859494</v>
+        <v>0.9646444442435405</v>
       </c>
       <c r="R18" t="n">
         <v>2827.0</v>
@@ -4422,16 +4422,16 @@
         <v>17294.0</v>
       </c>
       <c r="T18" t="n">
-        <v>0.8729798193838143</v>
+        <v>0.9042582651198517</v>
       </c>
       <c r="U18" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="V18" t="n">
-        <v>0.07303110905516363</v>
+        <v>0.07291546200994564</v>
       </c>
       <c r="W18" t="n">
-        <v>0.061292933965537186</v>
+        <v>0.05938475771944027</v>
       </c>
       <c r="X18" t="n">
         <v>8.0</v>
@@ -4440,7 +4440,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.9655392943333462</v>
+        <v>0.9655289228439817</v>
       </c>
       <c r="AA18" t="n">
         <v>2927.0</v>
@@ -4463,34 +4463,34 @@
         <v>0.0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.36340941512125535</v>
+        <v>0.3223965763195435</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5848787446504993</v>
+        <v>0.8309557774607703</v>
       </c>
       <c r="G19" t="n">
-        <v>0.6619115549215406</v>
+        <v>0.7942225392296719</v>
       </c>
       <c r="H19" t="n">
-        <v>0.6437232524964337</v>
+        <v>0.6483594864479315</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0010699001426533524</v>
+        <v>7.132667617689016E-4</v>
       </c>
       <c r="J19" t="n">
         <v>0.0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.8976654177026535</v>
+        <v>0.8905269355950052</v>
       </c>
       <c r="L19" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="M19" t="n">
-        <v>0.07742569677344743</v>
+        <v>0.07858216722562739</v>
       </c>
       <c r="N19" t="n">
-        <v>0.06800046258818088</v>
+        <v>0.06635249219382447</v>
       </c>
       <c r="O19" t="n">
         <v>8.0</v>
@@ -4499,7 +4499,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.964695742932859</v>
+        <v>0.9644770076124555</v>
       </c>
       <c r="R19" t="n">
         <v>2827.0</v>
@@ -4508,16 +4508,16 @@
         <v>17294.0</v>
       </c>
       <c r="T19" t="n">
-        <v>0.9211999693123131</v>
+        <v>0.9164430436532871</v>
       </c>
       <c r="U19" t="n">
-        <v>1.6448547923467098</v>
+        <v>1.6449558843640575</v>
       </c>
       <c r="V19" t="n">
-        <v>0.047241817971550824</v>
+        <v>0.04712617092633283</v>
       </c>
       <c r="W19" t="n">
-        <v>0.02503758528969585</v>
+        <v>0.024921938244477852</v>
       </c>
       <c r="X19" t="n">
         <v>8.0</v>
@@ -4526,7 +4526,7 @@
         <v>0.42796005706134094</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.9780908446309168</v>
+        <v>0.9782073990352628</v>
       </c>
       <c r="AA19" t="n">
         <v>2804.0</v>
@@ -4555,7 +4555,7 @@
         <v>8.0</v>
       </c>
       <c r="G20" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="H20" t="n">
         <v>8.0</v>
@@ -4567,16 +4567,16 @@
         <v>8.0</v>
       </c>
       <c r="K20" t="n">
-        <v>0.8976654177026535</v>
+        <v>0.8905269355950052</v>
       </c>
       <c r="L20" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="M20" t="n">
-        <v>0.07742569677344743</v>
+        <v>0.07858216722562739</v>
       </c>
       <c r="N20" t="n">
-        <v>0.06800046258818088</v>
+        <v>0.06635249219382447</v>
       </c>
       <c r="O20" t="n">
         <v>8.0</v>
@@ -4585,7 +4585,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.964695742932859</v>
+        <v>0.9644770076124555</v>
       </c>
       <c r="R20" t="n">
         <v>2827.0</v>
@@ -4594,16 +4594,16 @@
         <v>17294.0</v>
       </c>
       <c r="T20" t="n">
-        <v>0.9211999693123131</v>
+        <v>0.9164430436532871</v>
       </c>
       <c r="U20" t="n">
-        <v>1.6448547923467098</v>
+        <v>1.6449558843640575</v>
       </c>
       <c r="V20" t="n">
-        <v>0.047241817971550824</v>
+        <v>0.04712617092633283</v>
       </c>
       <c r="W20" t="n">
-        <v>0.02503758528969585</v>
+        <v>0.024921938244477852</v>
       </c>
       <c r="X20" t="n">
         <v>8.0</v>
@@ -4612,7 +4612,7 @@
         <v>0.42796005706134094</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.9780908446309168</v>
+        <v>0.9782073990352628</v>
       </c>
       <c r="AA20" t="n">
         <v>2804.0</v>
@@ -4635,34 +4635,34 @@
         <v>0.5492154065620543</v>
       </c>
       <c r="E21" t="n">
-        <v>0.36340941512125535</v>
+        <v>0.41298145506419404</v>
       </c>
       <c r="F21" t="n">
-        <v>0.5848787446504993</v>
+        <v>0.8309557774607703</v>
       </c>
       <c r="G21" t="n">
-        <v>0.6619115549215406</v>
+        <v>0.7942225392296719</v>
       </c>
       <c r="H21" t="n">
-        <v>0.6437232524964337</v>
+        <v>0.6483594864479315</v>
       </c>
       <c r="I21" t="n">
-        <v>0.5517118402282454</v>
+        <v>0.5470756062767475</v>
       </c>
       <c r="J21" t="n">
-        <v>0.4768188302425107</v>
+        <v>0.48858773181169757</v>
       </c>
       <c r="K21" t="n">
-        <v>0.8976654177026535</v>
+        <v>0.8905269355950052</v>
       </c>
       <c r="L21" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="M21" t="n">
-        <v>0.07742569677344743</v>
+        <v>0.07858216722562739</v>
       </c>
       <c r="N21" t="n">
-        <v>0.06800046258818088</v>
+        <v>0.06635249219382447</v>
       </c>
       <c r="O21" t="n">
         <v>8.0</v>
@@ -4671,7 +4671,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.964695742932859</v>
+        <v>0.9644770076124555</v>
       </c>
       <c r="R21" t="n">
         <v>2827.0</v>
@@ -4680,16 +4680,16 @@
         <v>17294.0</v>
       </c>
       <c r="T21" t="n">
-        <v>0.9211999693123131</v>
+        <v>0.9164430436532871</v>
       </c>
       <c r="U21" t="n">
-        <v>1.6448547923467098</v>
+        <v>1.6449558843640575</v>
       </c>
       <c r="V21" t="n">
-        <v>0.047241817971550824</v>
+        <v>0.04712617092633283</v>
       </c>
       <c r="W21" t="n">
-        <v>0.02503758528969585</v>
+        <v>0.024921938244477852</v>
       </c>
       <c r="X21" t="n">
         <v>8.0</v>
@@ -4698,7 +4698,7 @@
         <v>0.42796005706134094</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.9780908446309168</v>
+        <v>0.9782073990352628</v>
       </c>
       <c r="AA21" t="n">
         <v>2804.0</v>
@@ -4721,61 +4721,61 @@
         <v>0.0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.3160232319781346</v>
+        <v>0.30167406901264093</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4243252476938845</v>
+        <v>0.5066621113768364</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5155449265459515</v>
+        <v>0.49812094294499487</v>
       </c>
       <c r="H22" t="n">
-        <v>0.5644004099760848</v>
+        <v>0.5913905022207038</v>
       </c>
       <c r="I22" t="n">
-        <v>3.4164673727365904E-4</v>
+        <v>0.005466347796378545</v>
       </c>
       <c r="J22" t="n">
         <v>0.0</v>
       </c>
       <c r="K22" t="n">
-        <v>0.9221351017723327</v>
+        <v>0.9107468577455363</v>
       </c>
       <c r="L22" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6449992268231095</v>
       </c>
       <c r="M22" t="n">
-        <v>0.04758418740849195</v>
+        <v>0.04780943799977475</v>
       </c>
       <c r="N22" t="n">
-        <v>0.025791192701880843</v>
+        <v>0.02607275594098435</v>
       </c>
       <c r="O22" t="n">
         <v>8.0</v>
       </c>
       <c r="P22" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.42806140664048553</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.978323523908231</v>
+        <v>0.9782217217725766</v>
       </c>
       <c r="R22" t="n">
-        <v>2806.0</v>
+        <v>2801.0</v>
       </c>
       <c r="S22" t="n">
         <v>17758.0</v>
       </c>
       <c r="T22" t="n">
-        <v>0.8985035060941358</v>
+        <v>0.8761406687344427</v>
       </c>
       <c r="U22" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="V22" t="n">
-        <v>0.07039080977587567</v>
+        <v>0.07101024890190337</v>
       </c>
       <c r="W22" t="n">
-        <v>0.06062056537898412</v>
+        <v>0.06132447347674287</v>
       </c>
       <c r="X22" t="n">
         <v>8.0</v>
@@ -4784,7 +4784,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.9662221077799068</v>
+        <v>0.9663097608114993</v>
       </c>
       <c r="AA22" t="n">
         <v>2927.0</v>
@@ -4810,7 +4810,7 @@
         <v>8.0</v>
       </c>
       <c r="F23" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="G23" t="n">
         <v>9.0</v>
@@ -4825,43 +4825,43 @@
         <v>8.0</v>
       </c>
       <c r="K23" t="n">
-        <v>0.9221351017723327</v>
+        <v>0.9107468577455363</v>
       </c>
       <c r="L23" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6449992268231095</v>
       </c>
       <c r="M23" t="n">
-        <v>0.04758418740849195</v>
+        <v>0.04780943799977475</v>
       </c>
       <c r="N23" t="n">
-        <v>0.025791192701880843</v>
+        <v>0.02607275594098435</v>
       </c>
       <c r="O23" t="n">
         <v>8.0</v>
       </c>
       <c r="P23" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.42806140664048553</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.978323523908231</v>
+        <v>0.9782217217725766</v>
       </c>
       <c r="R23" t="n">
-        <v>2806.0</v>
+        <v>2801.0</v>
       </c>
       <c r="S23" t="n">
         <v>17758.0</v>
       </c>
       <c r="T23" t="n">
-        <v>0.8985035060941358</v>
+        <v>0.8761406687344427</v>
       </c>
       <c r="U23" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="V23" t="n">
-        <v>0.07039080977587567</v>
+        <v>0.07101024890190337</v>
       </c>
       <c r="W23" t="n">
-        <v>0.06062056537898412</v>
+        <v>0.06132447347674287</v>
       </c>
       <c r="X23" t="n">
         <v>8.0</v>
@@ -4870,7 +4870,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.9662221077799068</v>
+        <v>0.9663097608114993</v>
       </c>
       <c r="AA23" t="n">
         <v>2927.0</v>
@@ -4890,64 +4890,64 @@
         <v>47</v>
       </c>
       <c r="D24" t="n">
-        <v>0.36624530235736247</v>
+        <v>0.3703450632046464</v>
       </c>
       <c r="E24" t="n">
-        <v>0.417833959685685</v>
+        <v>0.4253501879057055</v>
       </c>
       <c r="F24" t="n">
-        <v>0.44140758455756746</v>
+        <v>0.5066621113768364</v>
       </c>
       <c r="G24" t="n">
-        <v>0.5155449265459515</v>
+        <v>0.49812094294499487</v>
       </c>
       <c r="H24" t="n">
-        <v>0.5644004099760848</v>
+        <v>0.5913905022207038</v>
       </c>
       <c r="I24" t="n">
-        <v>0.4151007857874957</v>
+        <v>0.41646737273659035</v>
       </c>
       <c r="J24" t="n">
-        <v>0.4314998291766314</v>
+        <v>0.44482405193030405</v>
       </c>
       <c r="K24" t="n">
-        <v>0.9221351017723327</v>
+        <v>0.9107468577455363</v>
       </c>
       <c r="L24" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6449992268231095</v>
       </c>
       <c r="M24" t="n">
-        <v>0.04758418740849195</v>
+        <v>0.04780943799977475</v>
       </c>
       <c r="N24" t="n">
-        <v>0.025791192701880843</v>
+        <v>0.02607275594098435</v>
       </c>
       <c r="O24" t="n">
         <v>8.0</v>
       </c>
       <c r="P24" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.42806140664048553</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.978323523908231</v>
+        <v>0.9782217217725766</v>
       </c>
       <c r="R24" t="n">
-        <v>2806.0</v>
+        <v>2801.0</v>
       </c>
       <c r="S24" t="n">
         <v>17758.0</v>
       </c>
       <c r="T24" t="n">
-        <v>0.8985035060941358</v>
+        <v>0.8761406687344427</v>
       </c>
       <c r="U24" t="n">
         <v>1.6408641369006336</v>
       </c>
       <c r="V24" t="n">
-        <v>0.07039080977587567</v>
+        <v>0.07101024890190337</v>
       </c>
       <c r="W24" t="n">
-        <v>0.06062056537898412</v>
+        <v>0.06132447347674287</v>
       </c>
       <c r="X24" t="n">
         <v>8.0</v>
@@ -4956,7 +4956,7 @@
         <v>0.4103177314656645</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.9662221077799068</v>
+        <v>0.9663097608114993</v>
       </c>
       <c r="AA24" t="n">
         <v>2927.0</v>
@@ -4979,43 +4979,43 @@
         <v>0.0</v>
       </c>
       <c r="E25" t="n">
-        <v>0.35514679872656524</v>
+        <v>0.40113194198797314</v>
       </c>
       <c r="F25" t="n">
-        <v>0.5298903431199151</v>
+        <v>0.5334276618323311</v>
       </c>
       <c r="G25" t="n">
-        <v>0.5935620799434029</v>
+        <v>0.597806862398302</v>
       </c>
       <c r="H25" t="n">
-        <v>0.8312698974177574</v>
+        <v>0.8857446055889636</v>
       </c>
       <c r="I25" t="n">
-        <v>0.005659709939865582</v>
+        <v>0.0017686593562079944</v>
       </c>
       <c r="J25" t="n">
         <v>0.0</v>
       </c>
       <c r="K25" t="n">
-        <v>0.9231524454132581</v>
+        <v>0.9029955643655834</v>
       </c>
       <c r="L25" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6451874590741786</v>
       </c>
       <c r="M25" t="n">
-        <v>0.0474434057889402</v>
+        <v>0.047837594323685104</v>
       </c>
       <c r="N25" t="n">
-        <v>0.02542516049104629</v>
+        <v>0.025833427187746373</v>
       </c>
       <c r="O25" t="n">
         <v>8.0</v>
       </c>
       <c r="P25" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.4280114041339986</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.9784063873875082</v>
+        <v>0.9781110971879238</v>
       </c>
       <c r="R25" t="n">
         <v>2806.0</v>
@@ -5024,16 +5024,16 @@
         <v>17758.0</v>
       </c>
       <c r="T25" t="n">
-        <v>0.9223087932910594</v>
+        <v>0.8825180346154053</v>
       </c>
       <c r="U25" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="V25" t="n">
-        <v>0.07664151368397341</v>
+        <v>0.0755715733753801</v>
       </c>
       <c r="W25" t="n">
-        <v>0.06180313098321884</v>
+        <v>0.06425273116341931</v>
       </c>
       <c r="X25" t="n">
         <v>8.0</v>
@@ -5042,7 +5042,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.9656281700763872</v>
+        <v>0.9657130473994732</v>
       </c>
       <c r="AA25" t="n">
         <v>2827.0</v>
@@ -5065,10 +5065,10 @@
         <v>8.0</v>
       </c>
       <c r="E26" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="F26" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="G26" t="n">
         <v>9.0</v>
@@ -5083,25 +5083,25 @@
         <v>8.0</v>
       </c>
       <c r="K26" t="n">
-        <v>0.9231524454132581</v>
+        <v>0.9029955643655834</v>
       </c>
       <c r="L26" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6451874590741786</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0474434057889402</v>
+        <v>0.047837594323685104</v>
       </c>
       <c r="N26" t="n">
-        <v>0.02542516049104629</v>
+        <v>0.025833427187746373</v>
       </c>
       <c r="O26" t="n">
         <v>8.0</v>
       </c>
       <c r="P26" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.4280114041339986</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.9784063873875082</v>
+        <v>0.9781110971879238</v>
       </c>
       <c r="R26" t="n">
         <v>2806.0</v>
@@ -5110,16 +5110,16 @@
         <v>17758.0</v>
       </c>
       <c r="T26" t="n">
-        <v>0.9223087932910594</v>
+        <v>0.8825180346154053</v>
       </c>
       <c r="U26" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="V26" t="n">
-        <v>0.07664151368397341</v>
+        <v>0.0755715733753801</v>
       </c>
       <c r="W26" t="n">
-        <v>0.06180313098321884</v>
+        <v>0.06425273116341931</v>
       </c>
       <c r="X26" t="n">
         <v>8.0</v>
@@ -5128,7 +5128,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Z26" t="n">
-        <v>0.9656281700763872</v>
+        <v>0.9657130473994732</v>
       </c>
       <c r="AA26" t="n">
         <v>2827.0</v>
@@ -5148,46 +5148,46 @@
         <v>47</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4082065794128051</v>
+        <v>0.43226034665723384</v>
       </c>
       <c r="E27" t="n">
-        <v>0.42553944110364345</v>
+        <v>0.43190661478599224</v>
       </c>
       <c r="F27" t="n">
-        <v>0.5298903431199151</v>
+        <v>0.5334276618323311</v>
       </c>
       <c r="G27" t="n">
-        <v>0.5935620799434029</v>
+        <v>0.597806862398302</v>
       </c>
       <c r="H27" t="n">
-        <v>0.8312698974177574</v>
+        <v>0.8857446055889636</v>
       </c>
       <c r="I27" t="n">
-        <v>0.4159886805801203</v>
+        <v>0.4170498761938451</v>
       </c>
       <c r="J27" t="n">
-        <v>0.4421648390519986</v>
+        <v>0.4386275203395826</v>
       </c>
       <c r="K27" t="n">
-        <v>0.9231524454132581</v>
+        <v>0.9029955643655834</v>
       </c>
       <c r="L27" t="n">
-        <v>1.6455504675603698</v>
+        <v>1.6451874590741786</v>
       </c>
       <c r="M27" t="n">
-        <v>0.0474434057889402</v>
+        <v>0.047837594323685104</v>
       </c>
       <c r="N27" t="n">
-        <v>0.02542516049104629</v>
+        <v>0.025833427187746373</v>
       </c>
       <c r="O27" t="n">
         <v>8.0</v>
       </c>
       <c r="P27" t="n">
-        <v>0.4276550249465431</v>
+        <v>0.4280114041339986</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.9784063873875082</v>
+        <v>0.9781110971879238</v>
       </c>
       <c r="R27" t="n">
         <v>2806.0</v>
@@ -5196,16 +5196,16 @@
         <v>17758.0</v>
       </c>
       <c r="T27" t="n">
-        <v>0.9223087932910594</v>
+        <v>0.8825180346154053</v>
       </c>
       <c r="U27" t="n">
         <v>1.6536120995775543</v>
       </c>
       <c r="V27" t="n">
-        <v>0.07664151368397341</v>
+        <v>0.0755715733753801</v>
       </c>
       <c r="W27" t="n">
-        <v>0.06180313098321884</v>
+        <v>0.06425273116341931</v>
       </c>
       <c r="X27" t="n">
         <v>8.0</v>
@@ -5214,7 +5214,7 @@
         <v>0.41740360806508664</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.9656281700763872</v>
+        <v>0.9657130473994732</v>
       </c>
       <c r="AA27" t="n">
         <v>2827.0</v>

</xml_diff>